<commit_message>
auto increment public id and fix unit tests
</commit_message>
<xml_diff>
--- a/resources/entity-sample-data/1. themes.xlsx
+++ b/resources/entity-sample-data/1. themes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Public ID</t>
   </si>
@@ -44,42 +44,6 @@
   </si>
   <si>
     <t>Description 4</t>
-  </si>
-  <si>
-    <t>Theme 5</t>
-  </si>
-  <si>
-    <t>Description 5</t>
-  </si>
-  <si>
-    <t>Theme 6</t>
-  </si>
-  <si>
-    <t>Description 6</t>
-  </si>
-  <si>
-    <t>Theme 7</t>
-  </si>
-  <si>
-    <t>Description 7</t>
-  </si>
-  <si>
-    <t>Theme 8</t>
-  </si>
-  <si>
-    <t>Description 8</t>
-  </si>
-  <si>
-    <t>Theme 9</t>
-  </si>
-  <si>
-    <t>Description 9</t>
-  </si>
-  <si>
-    <t>Theme 10</t>
-  </si>
-  <si>
-    <t>Description 10</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1464,9 +1428,7 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="4">
-        <v>3</v>
-      </c>
+      <c r="A2" s="4"/>
       <c r="B2" t="s" s="5">
         <v>3</v>
       </c>
@@ -1480,9 +1442,7 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="8">
-        <v>5</v>
-      </c>
+      <c r="A3" s="8"/>
       <c r="B3" t="s" s="9">
         <v>5</v>
       </c>
@@ -1496,9 +1456,7 @@
       <c r="H3" s="11"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="12">
-        <v>7</v>
-      </c>
+      <c r="A4" s="12"/>
       <c r="B4" t="s" s="13">
         <v>7</v>
       </c>
@@ -1512,9 +1470,7 @@
       <c r="H4" s="11"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="12">
-        <v>9</v>
-      </c>
+      <c r="A5" s="12"/>
       <c r="B5" t="s" s="13">
         <v>9</v>
       </c>
@@ -1528,15 +1484,9 @@
       <c r="H5" s="11"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="12">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s" s="13">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s" s="10">
-        <v>12</v>
-      </c>
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -1544,15 +1494,9 @@
       <c r="H6" s="11"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="12">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s" s="13">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s" s="10">
-        <v>14</v>
-      </c>
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -1560,15 +1504,9 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s" s="13">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s" s="10">
-        <v>16</v>
-      </c>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -1576,15 +1514,9 @@
       <c r="H8" s="11"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="12">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s" s="13">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s" s="10">
-        <v>18</v>
-      </c>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -1592,15 +1524,9 @@
       <c r="H9" s="11"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="12">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s" s="13">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s" s="10">
-        <v>20</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -1608,15 +1534,9 @@
       <c r="H10" s="11"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="12">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s" s="13">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s" s="10">
-        <v>22</v>
-      </c>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -1673,66 +1593,6 @@
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-    </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>